<commit_message>
updated IRRemote library + updated ir receiver - updated the system to use the latest version of the Arduino IRRemote  library.  The system previously used a fork of the library that added  esp32 send support, but esp32 send support has recently been merged  into the main library - because of this, the ir receiver thing doesn't break the system   anymore!  previously, once you started the IR receiver, it couldn't   be stopped, so you had to restart the system to do anything else   (including drawing to the screen) or the system would crash.  Now,   the ir receiver can be stopped, so you can receive IR, disable the   receiver, and do something else, without having to reset the system.   This also means that received codes can be written to the tft (rather   than needing to be printed over serial).
</commit_message>
<xml_diff>
--- a/extras/pinout.xlsx
+++ b/extras/pinout.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
   <si>
     <t xml:space="preserve">GND</t>
   </si>
@@ -55,45 +55,42 @@
     <t xml:space="preserve">dpad enter</t>
   </si>
   <si>
-    <t xml:space="preserve">TFT Backlight</t>
+    <t xml:space="preserve">Torch LED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IR LED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dpad down</t>
+  </si>
+  <si>
+    <t xml:space="preserve">screenshot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B (up)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D (down)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dpad up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dpad right</t>
   </si>
   <si>
     <t xml:space="preserve">SD CS</t>
   </si>
   <si>
-    <t xml:space="preserve">TX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dpad down</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IR LED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">screenshot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B (up)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D (down)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">battery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reset</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dpad right</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Torch LED</t>
-  </si>
-  <si>
     <t xml:space="preserve">dpad left</t>
   </si>
   <si>
@@ -106,7 +103,7 @@
     <t xml:space="preserve">Common</t>
   </si>
   <si>
-    <t xml:space="preserve">dpad up</t>
+    <t xml:space="preserve">TFT backlight</t>
   </si>
   <si>
     <t xml:space="preserve">Clock</t>
@@ -157,6 +154,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -178,15 +176,17 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -231,14 +231,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF006400"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF8A2BE2"/>
         <bgColor rgb="FF993366"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF006400"/>
-        <bgColor rgb="FF003300"/>
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
     <fill>
@@ -351,7 +357,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -380,6 +386,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -416,14 +426,18 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -452,14 +466,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -472,11 +486,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -563,9 +577,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>755640</xdr:colOff>
+      <xdr:colOff>754920</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>154080</xdr:rowOff>
+      <xdr:rowOff>153360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -578,8 +592,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8174520" y="4490280"/>
-          <a:ext cx="1521720" cy="1607400"/>
+          <a:off x="8200080" y="4490280"/>
+          <a:ext cx="1523520" cy="1606680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -602,7 +616,7 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>167400</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>110520</xdr:rowOff>
+      <xdr:rowOff>109800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -611,8 +625,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4230720" y="5679360"/>
-          <a:ext cx="360" cy="44280"/>
+          <a:off x="4243680" y="5679360"/>
+          <a:ext cx="360" cy="43560"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -644,9 +658,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>500400</xdr:colOff>
+      <xdr:colOff>499680</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>87840</xdr:rowOff>
+      <xdr:rowOff>87120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -655,8 +669,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1907280" y="4853880"/>
-          <a:ext cx="1031400" cy="1012320"/>
+          <a:off x="1912320" y="4853880"/>
+          <a:ext cx="1033200" cy="1011600"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -688,9 +702,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>302400</xdr:colOff>
+      <xdr:colOff>301680</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>121320</xdr:rowOff>
+      <xdr:rowOff>120600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -699,8 +713,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1647000" y="4644720"/>
-          <a:ext cx="280800" cy="264240"/>
+          <a:off x="1652040" y="4644720"/>
+          <a:ext cx="280080" cy="263520"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -732,9 +746,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>343800</xdr:colOff>
+      <xdr:colOff>343080</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>110160</xdr:rowOff>
+      <xdr:rowOff>109440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -743,8 +757,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1688400" y="5789520"/>
-          <a:ext cx="280800" cy="264240"/>
+          <a:off x="1693440" y="5789520"/>
+          <a:ext cx="280080" cy="263520"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -776,9 +790,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>729000</xdr:colOff>
+      <xdr:colOff>728280</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>99000</xdr:rowOff>
+      <xdr:rowOff>98280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -787,8 +801,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2886480" y="5778360"/>
-          <a:ext cx="280800" cy="264240"/>
+          <a:off x="2894040" y="5778360"/>
+          <a:ext cx="280080" cy="263520"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -820,9 +834,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>739080</xdr:colOff>
+      <xdr:colOff>738360</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>11160</xdr:rowOff>
+      <xdr:rowOff>10440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -831,8 +845,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2896560" y="4699800"/>
-          <a:ext cx="280800" cy="264240"/>
+          <a:off x="2904120" y="4699800"/>
+          <a:ext cx="280080" cy="263520"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -865,11 +879,11 @@
   </sheetPr>
   <dimension ref="B28:P48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N19" activeCellId="0" sqref="N19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L20" activeCellId="0" sqref="L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="28" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H28" s="1" t="s">
@@ -896,294 +910,292 @@
       <c r="H29" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="I29" s="0" t="s">
+      <c r="I29" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="J29" s="7" t="n">
+      <c r="J29" s="8" t="n">
         <v>26</v>
       </c>
-      <c r="M29" s="8" t="s">
+      <c r="M29" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="O29" s="9" t="n">
+      <c r="O29" s="10" t="n">
         <v>23</v>
       </c>
-      <c r="P29" s="10" t="s">
+      <c r="P29" s="11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="11"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="0" t="s">
+      <c r="C30" s="12"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H30" s="12" t="s">
+      <c r="H30" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="I30" s="0" t="s">
+      <c r="I30" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J30" s="7" t="n">
+      <c r="J30" s="8" t="n">
         <v>27</v>
       </c>
-      <c r="M30" s="8" t="s">
+      <c r="M30" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="O30" s="9" t="n">
+      <c r="O30" s="10" t="n">
         <v>22</v>
       </c>
-      <c r="P30" s="10" t="s">
+      <c r="P30" s="11" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="11"/>
-      <c r="D31" s="10"/>
-      <c r="G31" s="0" t="s">
+      <c r="C31" s="12"/>
+      <c r="D31" s="11"/>
+      <c r="G31" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H31" s="13" t="n">
+      <c r="H31" s="14" t="n">
         <v>36</v>
       </c>
-      <c r="I31" s="0" t="s">
+      <c r="I31" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="J31" s="9" t="n">
+      <c r="J31" s="15" t="n">
         <v>14</v>
       </c>
-      <c r="M31" s="9" t="n">
+      <c r="M31" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="N31" s="0" t="s">
+      <c r="N31" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="O31" s="14" t="n">
+      <c r="O31" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="P31" s="10" t="s">
+      <c r="P31" s="11" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="11"/>
-      <c r="D32" s="10"/>
-      <c r="G32" s="0" t="s">
+      <c r="C32" s="12"/>
+      <c r="D32" s="11"/>
+      <c r="G32" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="H32" s="13" t="n">
+      <c r="H32" s="14" t="n">
         <v>39</v>
       </c>
-      <c r="I32" s="0" t="s">
+      <c r="I32" s="7"/>
+      <c r="J32" s="17" t="n">
+        <v>12</v>
+      </c>
+      <c r="M32" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="N32" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="J32" s="15" t="n">
-        <v>12</v>
-      </c>
-      <c r="M32" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="N32" s="0" t="s">
+      <c r="O32" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="P32" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="O32" s="14" t="n">
-        <v>3</v>
-      </c>
-      <c r="P32" s="10" t="s">
+    </row>
+    <row r="33" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="33" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="0" t="s">
+      <c r="C33" s="12"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C33" s="11"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="0" t="s">
+      <c r="G33" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G33" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H33" s="16" t="n">
+      <c r="H33" s="18" t="n">
         <v>34</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M33" s="8" t="n">
+      <c r="M33" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="O33" s="9" t="n">
+      <c r="O33" s="10" t="n">
         <v>21</v>
       </c>
-      <c r="P33" s="10" t="s">
+      <c r="P33" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C34" s="12"/>
+      <c r="D34" s="11"/>
+      <c r="G34" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="34" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C34" s="11"/>
-      <c r="D34" s="10"/>
-      <c r="G34" s="0" t="s">
+      <c r="H34" s="14" t="n">
+        <v>35</v>
+      </c>
+      <c r="I34" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H34" s="13" t="n">
+      <c r="J34" s="10" t="n">
+        <v>13</v>
+      </c>
+      <c r="M34" s="9" t="n">
+        <v>15</v>
+      </c>
+      <c r="O34" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="P34" s="11"/>
+    </row>
+    <row r="35" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C35" s="12"/>
+      <c r="D35" s="11"/>
+      <c r="G35" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H35" s="14" t="n">
+        <v>32</v>
+      </c>
+      <c r="J35" s="19" t="n">
+        <v>9</v>
+      </c>
+      <c r="M35" s="19" t="n">
+        <v>8</v>
+      </c>
+      <c r="O35" s="10" t="n">
+        <v>19</v>
+      </c>
+      <c r="P35" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C36" s="12"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H36" s="10" t="n">
+        <v>33</v>
+      </c>
+      <c r="J36" s="19" t="n">
+        <v>10</v>
+      </c>
+      <c r="M36" s="19" t="n">
+        <v>7</v>
+      </c>
+      <c r="O36" s="10" t="n">
+        <v>18</v>
+      </c>
+      <c r="P36" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C37" s="20"/>
+      <c r="D37" s="21"/>
+      <c r="G37" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H37" s="8" t="n">
+        <v>25</v>
+      </c>
+      <c r="I37" s="22"/>
+      <c r="J37" s="19" t="n">
+        <v>11</v>
+      </c>
+      <c r="K37" s="22"/>
+      <c r="L37" s="22"/>
+      <c r="M37" s="19" t="n">
+        <v>6</v>
+      </c>
+      <c r="N37" s="22"/>
+      <c r="O37" s="10" t="n">
+        <v>5</v>
+      </c>
+      <c r="P37" s="21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="H39" s="24"/>
+      <c r="I39" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H40" s="25"/>
+      <c r="I40" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H41" s="26"/>
+      <c r="I41" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H42" s="27"/>
+      <c r="I42" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H43" s="28"/>
+      <c r="I43" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H44" s="29"/>
+      <c r="I44" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="I34" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="J34" s="15" t="n">
-        <v>13</v>
-      </c>
-      <c r="M34" s="8" t="n">
-        <v>15</v>
-      </c>
-      <c r="O34" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="P34" s="10"/>
-    </row>
-    <row r="35" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C35" s="11"/>
-      <c r="D35" s="10"/>
-      <c r="G35" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="H35" s="13" t="n">
-        <v>32</v>
-      </c>
-      <c r="J35" s="17" t="n">
-        <v>9</v>
-      </c>
-      <c r="M35" s="17" t="n">
-        <v>8</v>
-      </c>
-      <c r="O35" s="9" t="n">
-        <v>19</v>
-      </c>
-      <c r="P35" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C36" s="11"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="G36" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="H36" s="13" t="n">
-        <v>33</v>
-      </c>
-      <c r="J36" s="17" t="n">
-        <v>10</v>
-      </c>
-      <c r="M36" s="17" t="n">
-        <v>7</v>
-      </c>
-      <c r="O36" s="9" t="n">
-        <v>18</v>
-      </c>
-      <c r="P36" s="10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C37" s="18"/>
-      <c r="D37" s="19"/>
-      <c r="G37" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="H37" s="7" t="n">
-        <v>25</v>
-      </c>
-      <c r="I37" s="20"/>
-      <c r="J37" s="17" t="n">
-        <v>11</v>
-      </c>
-      <c r="K37" s="20"/>
-      <c r="L37" s="20"/>
-      <c r="M37" s="17" t="n">
-        <v>6</v>
-      </c>
-      <c r="N37" s="20"/>
-      <c r="O37" s="9" t="n">
-        <v>5</v>
-      </c>
-      <c r="P37" s="19" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="13.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="H39" s="22"/>
-      <c r="I39" s="0" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H40" s="23"/>
-      <c r="I40" s="0" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H41" s="24"/>
-      <c r="I41" s="0" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H42" s="25"/>
-      <c r="I42" s="0" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H43" s="26"/>
-      <c r="I43" s="0" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H44" s="27"/>
-      <c r="I44" s="0" t="s">
+    </row>
+    <row r="45" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H45" s="30"/>
+      <c r="I45" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H45" s="28"/>
-      <c r="I45" s="0" t="s">
+    <row r="46" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H46" s="31"/>
+      <c r="I46" s="7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H46" s="29"/>
-      <c r="I46" s="0" t="s">
+    <row r="47" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H47" s="32"/>
+      <c r="I47" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H47" s="30"/>
-      <c r="I47" s="0" t="s">
+    <row r="48" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H48" s="33"/>
+      <c r="I48" s="7" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H48" s="31"/>
-      <c r="I48" s="0" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated system to esp-idf-v4.0.1 and added jtag pins to pinout
</commit_message>
<xml_diff>
--- a/extras/pinout.xlsx
+++ b/extras/pinout.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
   <si>
     <t xml:space="preserve">GND</t>
   </si>
@@ -55,7 +55,25 @@
     <t xml:space="preserve">dpad enter</t>
   </si>
   <si>
-    <t xml:space="preserve">Torch LED</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Torch / </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">TMS</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">IR LED</t>
@@ -67,6 +85,9 @@
     <t xml:space="preserve">dpad down</t>
   </si>
   <si>
+    <t xml:space="preserve">TDI</t>
+  </si>
+  <si>
     <t xml:space="preserve">screenshot</t>
   </si>
   <si>
@@ -88,7 +109,28 @@
     <t xml:space="preserve">dpad right</t>
   </si>
   <si>
-    <t xml:space="preserve">SD CS</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">SD CS / </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">TCK</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">TDO</t>
   </si>
   <si>
     <t xml:space="preserve">dpad left</t>
@@ -149,7 +191,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -174,6 +216,13 @@
     <font>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -357,7 +406,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -426,6 +475,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -450,7 +503,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -577,9 +630,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>754920</xdr:colOff>
+      <xdr:colOff>754560</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>153360</xdr:rowOff>
+      <xdr:rowOff>134280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -592,8 +645,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8200080" y="4490280"/>
-          <a:ext cx="1523520" cy="1606680"/>
+          <a:off x="8212680" y="4490280"/>
+          <a:ext cx="1524240" cy="1606320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -610,13 +663,13 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>167040</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>66240</xdr:rowOff>
+      <xdr:rowOff>47160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>167400</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>109800</xdr:rowOff>
+      <xdr:rowOff>90360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -625,8 +678,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4243680" y="5679360"/>
-          <a:ext cx="360" cy="43560"/>
+          <a:off x="4249800" y="5679360"/>
+          <a:ext cx="360" cy="43200"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -658,9 +711,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>499680</xdr:colOff>
+      <xdr:colOff>499320</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>87120</xdr:rowOff>
+      <xdr:rowOff>67680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -669,8 +722,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1912320" y="4853880"/>
-          <a:ext cx="1033200" cy="1011600"/>
+          <a:off x="1914840" y="4853880"/>
+          <a:ext cx="1034280" cy="1011240"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -702,9 +755,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>301680</xdr:colOff>
+      <xdr:colOff>301320</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>120600</xdr:rowOff>
+      <xdr:rowOff>120240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -713,8 +766,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1652040" y="4644720"/>
-          <a:ext cx="280080" cy="263520"/>
+          <a:off x="1654560" y="4644720"/>
+          <a:ext cx="279720" cy="263160"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -741,14 +794,14 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>63000</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>11160</xdr:rowOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>157320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>343080</xdr:colOff>
+      <xdr:colOff>342720</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>109440</xdr:rowOff>
+      <xdr:rowOff>90360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -757,8 +810,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1693440" y="5789520"/>
-          <a:ext cx="280080" cy="263520"/>
+          <a:off x="1695960" y="5789520"/>
+          <a:ext cx="279720" cy="263160"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -785,14 +838,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>448200</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>146160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>728280</xdr:colOff>
+      <xdr:colOff>727920</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>98280</xdr:rowOff>
+      <xdr:rowOff>79200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -801,8 +854,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2894040" y="5778360"/>
-          <a:ext cx="280080" cy="263520"/>
+          <a:off x="2898000" y="5778360"/>
+          <a:ext cx="279720" cy="263160"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -834,9 +887,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>738360</xdr:colOff>
+      <xdr:colOff>738000</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>10440</xdr:rowOff>
+      <xdr:rowOff>10080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -845,8 +898,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2904120" y="4699800"/>
-          <a:ext cx="280080" cy="263520"/>
+          <a:off x="2908080" y="4699800"/>
+          <a:ext cx="279720" cy="263160"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -879,11 +932,11 @@
   </sheetPr>
   <dimension ref="B28:P48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J24" activeCellId="0" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="28" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H28" s="1" t="s">
@@ -954,7 +1007,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="12"/>
       <c r="D31" s="11"/>
       <c r="G31" s="7" t="s">
@@ -991,36 +1044,38 @@
       <c r="H32" s="14" t="n">
         <v>39</v>
       </c>
-      <c r="I32" s="7"/>
-      <c r="J32" s="17" t="n">
+      <c r="I32" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="J32" s="18" t="n">
         <v>12</v>
       </c>
       <c r="M32" s="13" t="n">
         <v>0</v>
       </c>
       <c r="N32" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O32" s="16" t="n">
         <v>3</v>
       </c>
       <c r="P32" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C33" s="12"/>
       <c r="D33" s="11"/>
       <c r="E33" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H33" s="18" t="n">
+        <v>20</v>
+      </c>
+      <c r="H33" s="19" t="n">
         <v>34</v>
       </c>
       <c r="J33" s="1" t="s">
@@ -1033,26 +1088,29 @@
         <v>21</v>
       </c>
       <c r="P33" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="12"/>
       <c r="D34" s="11"/>
       <c r="G34" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H34" s="14" t="n">
         <v>35</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J34" s="10" t="n">
         <v>13</v>
       </c>
       <c r="M34" s="9" t="n">
         <v>15</v>
+      </c>
+      <c r="N34" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="O34" s="9" t="s">
         <v>3</v>
@@ -1063,139 +1121,139 @@
       <c r="C35" s="12"/>
       <c r="D35" s="11"/>
       <c r="G35" s="7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H35" s="14" t="n">
         <v>32</v>
       </c>
-      <c r="J35" s="19" t="n">
+      <c r="J35" s="20" t="n">
         <v>9</v>
       </c>
-      <c r="M35" s="19" t="n">
+      <c r="M35" s="20" t="n">
         <v>8</v>
       </c>
       <c r="O35" s="10" t="n">
         <v>19</v>
       </c>
       <c r="P35" s="11" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C36" s="12"/>
       <c r="D36" s="11"/>
       <c r="E36" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H36" s="10" t="n">
         <v>33</v>
       </c>
-      <c r="J36" s="19" t="n">
+      <c r="J36" s="20" t="n">
         <v>10</v>
       </c>
-      <c r="M36" s="19" t="n">
+      <c r="M36" s="20" t="n">
         <v>7</v>
       </c>
       <c r="O36" s="10" t="n">
         <v>18</v>
       </c>
       <c r="P36" s="11" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C37" s="20"/>
-      <c r="D37" s="21"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="22"/>
       <c r="G37" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H37" s="8" t="n">
         <v>25</v>
       </c>
-      <c r="I37" s="22"/>
-      <c r="J37" s="19" t="n">
+      <c r="I37" s="23"/>
+      <c r="J37" s="20" t="n">
         <v>11</v>
       </c>
-      <c r="K37" s="22"/>
-      <c r="L37" s="22"/>
-      <c r="M37" s="19" t="n">
+      <c r="K37" s="23"/>
+      <c r="L37" s="23"/>
+      <c r="M37" s="20" t="n">
         <v>6</v>
       </c>
-      <c r="N37" s="22"/>
+      <c r="N37" s="23"/>
       <c r="O37" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="P37" s="21" t="s">
-        <v>30</v>
+      <c r="P37" s="22" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H39" s="24"/>
+      <c r="B39" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="H39" s="25"/>
       <c r="I39" s="7" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H40" s="25"/>
+      <c r="H40" s="26"/>
       <c r="I40" s="7" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H41" s="26"/>
+      <c r="H41" s="27"/>
       <c r="I41" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H42" s="27"/>
+      <c r="H42" s="28"/>
       <c r="I42" s="7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H43" s="28"/>
+      <c r="H43" s="29"/>
       <c r="I43" s="7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H44" s="29"/>
+      <c r="H44" s="30"/>
       <c r="I44" s="7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H45" s="30"/>
+      <c r="H45" s="31"/>
       <c r="I45" s="7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H46" s="31"/>
+      <c r="H46" s="32"/>
       <c r="I46" s="7" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H47" s="32"/>
+      <c r="H47" s="33"/>
       <c r="I47" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H48" s="33"/>
+      <c r="H48" s="34"/>
       <c r="I48" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more attempting to get music stuff working
</commit_message>
<xml_diff>
--- a/extras/pinout.xlsx
+++ b/extras/pinout.xlsx
@@ -85,7 +85,25 @@
     <t xml:space="preserve">dpad down</t>
   </si>
   <si>
-    <t xml:space="preserve">TDI</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">IR recv/</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">TDI</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">screenshot</t>
@@ -235,7 +253,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -288,12 +306,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF8A2BE2"/>
         <bgColor rgb="FF993366"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
     <fill>
@@ -406,7 +418,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -475,6 +487,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -483,14 +499,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -519,11 +527,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -630,9 +638,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>754560</xdr:colOff>
+      <xdr:colOff>753840</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>134280</xdr:rowOff>
+      <xdr:rowOff>136080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -645,13 +653,13 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8212680" y="4490280"/>
-          <a:ext cx="1524240" cy="1606320"/>
+          <a:off x="8238240" y="4490280"/>
+          <a:ext cx="1526040" cy="1605600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -663,13 +671,13 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>167040</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>47160</xdr:rowOff>
+      <xdr:rowOff>49680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>167400</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>90360</xdr:rowOff>
+      <xdr:rowOff>92160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -678,8 +686,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4249800" y="5679360"/>
-          <a:ext cx="360" cy="43200"/>
+          <a:off x="4262760" y="5679360"/>
+          <a:ext cx="360" cy="42480"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -687,7 +695,7 @@
         <a:solidFill>
           <a:srgbClr val="729fcf"/>
         </a:solidFill>
-        <a:ln>
+        <a:ln w="0">
           <a:solidFill>
             <a:srgbClr val="3465a4"/>
           </a:solidFill>
@@ -711,9 +719,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>499320</xdr:colOff>
+      <xdr:colOff>498600</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>67680</xdr:rowOff>
+      <xdr:rowOff>69480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -722,8 +730,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1914840" y="4853880"/>
-          <a:ext cx="1034280" cy="1011240"/>
+          <a:off x="1919880" y="4853880"/>
+          <a:ext cx="1036080" cy="1010520"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -731,7 +739,7 @@
         <a:solidFill>
           <a:srgbClr val="000000"/>
         </a:solidFill>
-        <a:ln>
+        <a:ln w="0">
           <a:solidFill>
             <a:srgbClr val="3465a4"/>
           </a:solidFill>
@@ -755,9 +763,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>301320</xdr:colOff>
+      <xdr:colOff>300600</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>120240</xdr:rowOff>
+      <xdr:rowOff>119520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -766,8 +774,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1654560" y="4644720"/>
-          <a:ext cx="279720" cy="263160"/>
+          <a:off x="1659600" y="4644720"/>
+          <a:ext cx="279000" cy="262440"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -775,7 +783,7 @@
         <a:solidFill>
           <a:srgbClr val="000000"/>
         </a:solidFill>
-        <a:ln>
+        <a:ln w="0">
           <a:solidFill>
             <a:srgbClr val="3465a4"/>
           </a:solidFill>
@@ -795,13 +803,13 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>63000</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>157320</xdr:rowOff>
+      <xdr:rowOff>159840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>342720</xdr:colOff>
+      <xdr:colOff>342000</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>90360</xdr:rowOff>
+      <xdr:rowOff>92160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -810,8 +818,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1695960" y="5789520"/>
-          <a:ext cx="279720" cy="263160"/>
+          <a:off x="1701000" y="5789520"/>
+          <a:ext cx="279000" cy="262440"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -819,7 +827,7 @@
         <a:solidFill>
           <a:srgbClr val="000000"/>
         </a:solidFill>
-        <a:ln>
+        <a:ln w="0">
           <a:solidFill>
             <a:srgbClr val="3465a4"/>
           </a:solidFill>
@@ -839,13 +847,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>448200</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>146160</xdr:rowOff>
+      <xdr:rowOff>148680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>727920</xdr:colOff>
+      <xdr:colOff>727200</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>79200</xdr:rowOff>
+      <xdr:rowOff>81000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -854,8 +862,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2898000" y="5778360"/>
-          <a:ext cx="279720" cy="263160"/>
+          <a:off x="2905560" y="5778360"/>
+          <a:ext cx="279000" cy="262440"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -863,7 +871,7 @@
         <a:solidFill>
           <a:srgbClr val="000000"/>
         </a:solidFill>
-        <a:ln>
+        <a:ln w="0">
           <a:solidFill>
             <a:srgbClr val="3465a4"/>
           </a:solidFill>
@@ -887,9 +895,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>738000</xdr:colOff>
+      <xdr:colOff>737280</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>10080</xdr:rowOff>
+      <xdr:rowOff>9360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -898,8 +906,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2908080" y="4699800"/>
-          <a:ext cx="279720" cy="263160"/>
+          <a:off x="2915640" y="4699800"/>
+          <a:ext cx="279000" cy="262440"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -907,7 +915,7 @@
         <a:solidFill>
           <a:srgbClr val="000000"/>
         </a:solidFill>
-        <a:ln>
+        <a:ln w="0">
           <a:solidFill>
             <a:srgbClr val="3465a4"/>
           </a:solidFill>
@@ -933,10 +941,10 @@
   <dimension ref="B28:P48"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J24" activeCellId="0" sqref="J24"/>
+      <selection pane="topLeft" activeCell="M34" activeCellId="0" sqref="M34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="28" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H28" s="1" t="s">
@@ -1035,7 +1043,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="12"/>
       <c r="D32" s="11"/>
       <c r="G32" s="7" t="s">
@@ -1044,12 +1052,10 @@
       <c r="H32" s="14" t="n">
         <v>39</v>
       </c>
-      <c r="I32" s="17" t="s">
+      <c r="I32" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="J32" s="18" t="n">
-        <v>12</v>
-      </c>
+      <c r="J32" s="15"/>
       <c r="M32" s="13" t="n">
         <v>0</v>
       </c>
@@ -1075,7 +1081,7 @@
       <c r="G33" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H33" s="19" t="n">
+      <c r="H33" s="17" t="n">
         <v>34</v>
       </c>
       <c r="J33" s="1" t="s">
@@ -1109,7 +1115,7 @@
       <c r="M34" s="9" t="n">
         <v>15</v>
       </c>
-      <c r="N34" s="17" t="s">
+      <c r="N34" s="18" t="s">
         <v>24</v>
       </c>
       <c r="O34" s="9" t="s">
@@ -1126,10 +1132,10 @@
       <c r="H35" s="14" t="n">
         <v>32</v>
       </c>
-      <c r="J35" s="20" t="n">
+      <c r="J35" s="19" t="n">
         <v>9</v>
       </c>
-      <c r="M35" s="20" t="n">
+      <c r="M35" s="19" t="n">
         <v>8</v>
       </c>
       <c r="O35" s="10" t="n">
@@ -1154,10 +1160,10 @@
       <c r="H36" s="10" t="n">
         <v>33</v>
       </c>
-      <c r="J36" s="20" t="n">
+      <c r="J36" s="19" t="n">
         <v>10</v>
       </c>
-      <c r="M36" s="20" t="n">
+      <c r="M36" s="19" t="n">
         <v>7</v>
       </c>
       <c r="O36" s="10" t="n">
@@ -1168,90 +1174,90 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C37" s="21"/>
-      <c r="D37" s="22"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="21"/>
       <c r="G37" s="7" t="s">
         <v>31</v>
       </c>
       <c r="H37" s="8" t="n">
         <v>25</v>
       </c>
-      <c r="I37" s="23"/>
-      <c r="J37" s="20" t="n">
+      <c r="I37" s="22"/>
+      <c r="J37" s="19" t="n">
         <v>11</v>
       </c>
-      <c r="K37" s="23"/>
-      <c r="L37" s="23"/>
-      <c r="M37" s="20" t="n">
+      <c r="K37" s="22"/>
+      <c r="L37" s="22"/>
+      <c r="M37" s="19" t="n">
         <v>6</v>
       </c>
-      <c r="N37" s="23"/>
+      <c r="N37" s="22"/>
       <c r="O37" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="P37" s="22" t="s">
+      <c r="P37" s="21" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="24" t="s">
+      <c r="B39" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="H39" s="25"/>
+      <c r="H39" s="24"/>
       <c r="I39" s="7" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H40" s="26"/>
+      <c r="H40" s="25"/>
       <c r="I40" s="7" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H41" s="27"/>
+      <c r="H41" s="26"/>
       <c r="I41" s="7" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H42" s="28"/>
+      <c r="H42" s="27"/>
       <c r="I42" s="7" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H43" s="29"/>
+      <c r="H43" s="28"/>
       <c r="I43" s="7" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H44" s="30"/>
+      <c r="H44" s="29"/>
       <c r="I44" s="7" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H45" s="31"/>
+      <c r="H45" s="30"/>
       <c r="I45" s="7" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H46" s="32"/>
+      <c r="H46" s="31"/>
       <c r="I46" s="7" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H47" s="33"/>
+      <c r="H47" s="32"/>
       <c r="I47" s="7" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H48" s="34"/>
+      <c r="H48" s="33"/>
       <c r="I48" s="7" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
file select menus now have icons!
</commit_message>
<xml_diff>
--- a/extras/pinout.xlsx
+++ b/extras/pinout.xlsx
@@ -106,7 +106,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">screenshot</t>
+    <t xml:space="preserve">SDA</t>
   </si>
   <si>
     <t xml:space="preserve">RX</t>
@@ -148,7 +148,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">TDO</t>
+    <t xml:space="preserve">SCL</t>
   </si>
   <si>
     <t xml:space="preserve">dpad left</t>
@@ -310,14 +310,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00CED1"/>
-        <bgColor rgb="FF33CCCC"/>
+        <fgColor rgb="FFFF1493"/>
+        <bgColor rgb="FFFF00FF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF1493"/>
-        <bgColor rgb="FFFF00FF"/>
+        <fgColor rgb="FF00CED1"/>
+        <bgColor rgb="FF33CCCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -418,7 +418,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -491,11 +491,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -527,11 +531,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -638,9 +642,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>753840</xdr:colOff>
+      <xdr:colOff>753480</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>136080</xdr:rowOff>
+      <xdr:rowOff>135720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -653,8 +657,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8238240" y="4490280"/>
-          <a:ext cx="1526040" cy="1605600"/>
+          <a:off x="8250840" y="4490280"/>
+          <a:ext cx="1527120" cy="1605240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -677,7 +681,7 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>167400</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>92160</xdr:rowOff>
+      <xdr:rowOff>91800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -686,8 +690,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4262760" y="5679360"/>
-          <a:ext cx="360" cy="42480"/>
+          <a:off x="4268880" y="5679360"/>
+          <a:ext cx="360" cy="42120"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -719,9 +723,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>498600</xdr:colOff>
+      <xdr:colOff>498240</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>69480</xdr:rowOff>
+      <xdr:rowOff>69120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -730,8 +734,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1919880" y="4853880"/>
-          <a:ext cx="1036080" cy="1010520"/>
+          <a:off x="1922400" y="4853880"/>
+          <a:ext cx="1036800" cy="1010160"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -763,9 +767,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>300600</xdr:colOff>
+      <xdr:colOff>300240</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>119520</xdr:rowOff>
+      <xdr:rowOff>119160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -774,8 +778,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1659600" y="4644720"/>
-          <a:ext cx="279000" cy="262440"/>
+          <a:off x="1662120" y="4644720"/>
+          <a:ext cx="278640" cy="262080"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -807,9 +811,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>342000</xdr:colOff>
+      <xdr:colOff>341640</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>92160</xdr:rowOff>
+      <xdr:rowOff>91800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -818,8 +822,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1701000" y="5789520"/>
-          <a:ext cx="279000" cy="262440"/>
+          <a:off x="1703520" y="5789520"/>
+          <a:ext cx="278640" cy="262080"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -851,9 +855,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>727200</xdr:colOff>
+      <xdr:colOff>726840</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>81000</xdr:rowOff>
+      <xdr:rowOff>80640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -862,8 +866,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2905560" y="5778360"/>
-          <a:ext cx="279000" cy="262440"/>
+          <a:off x="2909160" y="5778360"/>
+          <a:ext cx="278640" cy="262080"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -895,9 +899,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>737280</xdr:colOff>
+      <xdr:colOff>736920</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>9360</xdr:rowOff>
+      <xdr:rowOff>9000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -906,8 +910,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2915640" y="4699800"/>
-          <a:ext cx="279000" cy="262440"/>
+          <a:off x="2919240" y="4699800"/>
+          <a:ext cx="278640" cy="262080"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -940,11 +944,11 @@
   </sheetPr>
   <dimension ref="B28:P48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M34" activeCellId="0" sqref="M34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N32" activeCellId="0" sqref="N32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="28" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H28" s="1" t="s">
@@ -1055,7 +1059,9 @@
       <c r="I32" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="J32" s="15"/>
+      <c r="J32" s="15" t="n">
+        <v>12</v>
+      </c>
       <c r="M32" s="13" t="n">
         <v>0</v>
       </c>
@@ -1087,7 +1093,7 @@
       <c r="J33" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M33" s="9" t="n">
+      <c r="M33" s="18" t="n">
         <v>2</v>
       </c>
       <c r="O33" s="10" t="n">
@@ -1112,10 +1118,10 @@
       <c r="J34" s="10" t="n">
         <v>13</v>
       </c>
-      <c r="M34" s="9" t="n">
+      <c r="M34" s="18" t="n">
         <v>15</v>
       </c>
-      <c r="N34" s="18" t="s">
+      <c r="N34" s="19" t="s">
         <v>24</v>
       </c>
       <c r="O34" s="9" t="s">
@@ -1132,10 +1138,10 @@
       <c r="H35" s="14" t="n">
         <v>32</v>
       </c>
-      <c r="J35" s="19" t="n">
+      <c r="J35" s="20" t="n">
         <v>9</v>
       </c>
-      <c r="M35" s="19" t="n">
+      <c r="M35" s="20" t="n">
         <v>8</v>
       </c>
       <c r="O35" s="10" t="n">
@@ -1160,10 +1166,10 @@
       <c r="H36" s="10" t="n">
         <v>33</v>
       </c>
-      <c r="J36" s="19" t="n">
+      <c r="J36" s="20" t="n">
         <v>10</v>
       </c>
-      <c r="M36" s="19" t="n">
+      <c r="M36" s="20" t="n">
         <v>7</v>
       </c>
       <c r="O36" s="10" t="n">
@@ -1174,90 +1180,90 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C37" s="20"/>
-      <c r="D37" s="21"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="22"/>
       <c r="G37" s="7" t="s">
         <v>31</v>
       </c>
       <c r="H37" s="8" t="n">
         <v>25</v>
       </c>
-      <c r="I37" s="22"/>
-      <c r="J37" s="19" t="n">
+      <c r="I37" s="23"/>
+      <c r="J37" s="20" t="n">
         <v>11</v>
       </c>
-      <c r="K37" s="22"/>
-      <c r="L37" s="22"/>
-      <c r="M37" s="19" t="n">
+      <c r="K37" s="23"/>
+      <c r="L37" s="23"/>
+      <c r="M37" s="20" t="n">
         <v>6</v>
       </c>
-      <c r="N37" s="22"/>
+      <c r="N37" s="23"/>
       <c r="O37" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="P37" s="21" t="s">
+      <c r="P37" s="22" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="23" t="s">
+      <c r="B39" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="H39" s="24"/>
+      <c r="H39" s="25"/>
       <c r="I39" s="7" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H40" s="25"/>
+      <c r="H40" s="26"/>
       <c r="I40" s="7" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H41" s="26"/>
+      <c r="H41" s="27"/>
       <c r="I41" s="7" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H42" s="27"/>
+      <c r="H42" s="28"/>
       <c r="I42" s="7" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H43" s="28"/>
+      <c r="H43" s="29"/>
       <c r="I43" s="7" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H44" s="29"/>
+      <c r="H44" s="30"/>
       <c r="I44" s="7" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H45" s="30"/>
+      <c r="H45" s="31"/>
       <c r="I45" s="7" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H46" s="31"/>
+      <c r="H46" s="32"/>
       <c r="I46" s="7" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H47" s="32"/>
+      <c r="H47" s="33"/>
       <c r="I47" s="7" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H48" s="33"/>
+      <c r="H48" s="34"/>
       <c r="I48" s="7" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
moved dpad pins to external MCP23008 instead of wiring dpad pins to the esp32 (using 5 pins), they are now wired to an MCP23008 i2s io expander.  this means that there are now 5 more free pins on the esp32 (that i really need).  the mcp23008 has 3 leftover pins which is cool also, you can't wake up from sleep anymore
</commit_message>
<xml_diff>
--- a/extras/pinout.xlsx
+++ b/extras/pinout.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
   <si>
     <t xml:space="preserve">GND</t>
   </si>
@@ -50,9 +50,6 @@
   </si>
   <si>
     <t xml:space="preserve">DC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dpad enter</t>
   </si>
   <si>
     <r>
@@ -82,9 +79,6 @@
     <t xml:space="preserve">TX</t>
   </si>
   <si>
-    <t xml:space="preserve">dpad down</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="10"/>
@@ -106,9 +100,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">SDA</t>
-  </si>
-  <si>
     <t xml:space="preserve">RX</t>
   </si>
   <si>
@@ -118,13 +109,7 @@
     <t xml:space="preserve">D (down)</t>
   </si>
   <si>
-    <t xml:space="preserve">dpad up</t>
-  </si>
-  <si>
     <t xml:space="preserve">reset</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dpad right</t>
   </si>
   <si>
     <r>
@@ -151,49 +136,88 @@
     <t xml:space="preserve">SCL</t>
   </si>
   <si>
+    <t xml:space="preserve">SDA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MISO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C (left)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Common</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TFT backlight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I2S DOUT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TFT CS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://cdn-shop.adafruit.com/datasheets/SKQUCAA010-ALPS.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GP7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GP6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bootstrapping pins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GP5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Internal SPI pins (don’t use)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GP4</t>
+  </si>
+  <si>
     <t xml:space="preserve">dpad left</t>
   </si>
   <si>
-    <t xml:space="preserve">MISO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C (left)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Common</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TFT backlight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clock</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I2S DOUT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TFT CS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://cdn-shop.adafruit.com/datasheets/SKQUCAA010-ALPS.pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bootstrapping pins</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Internal SPI pins (don’t use)</t>
-  </si>
-  <si>
     <t xml:space="preserve">I2C</t>
   </si>
   <si>
+    <t xml:space="preserve">GP3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dpad down</t>
+  </si>
+  <si>
     <t xml:space="preserve">I2S</t>
   </si>
   <si>
+    <t xml:space="preserve">GP2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dpad enter</t>
+  </si>
+  <si>
     <t xml:space="preserve">VSPI + TFT stuff</t>
   </si>
   <si>
+    <t xml:space="preserve">GP1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dpad up</t>
+  </si>
+  <si>
     <t xml:space="preserve">dpad pins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GP0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dpad right</t>
   </si>
   <si>
     <t xml:space="preserve">other peripherals</t>
@@ -209,7 +233,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -239,6 +263,13 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <i val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
@@ -253,7 +284,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -292,8 +323,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF0000FF"/>
-        <bgColor rgb="FF0000FF"/>
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
     <fill>
@@ -318,6 +349,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF00CED1"/>
         <bgColor rgb="FF33CCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0000FF"/>
+        <bgColor rgb="FF0000FF"/>
       </patternFill>
     </fill>
   </fills>
@@ -418,7 +455,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -475,7 +512,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -487,16 +524,16 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -515,7 +552,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -523,6 +560,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -535,6 +576,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -547,7 +592,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -642,9 +687,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>753480</xdr:colOff>
+      <xdr:colOff>753120</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>135720</xdr:rowOff>
+      <xdr:rowOff>164520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -657,8 +702,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8250840" y="4490280"/>
-          <a:ext cx="1527120" cy="1605240"/>
+          <a:off x="8263440" y="4490280"/>
+          <a:ext cx="1528200" cy="1604880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -675,13 +720,13 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>167040</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>49680</xdr:rowOff>
+      <xdr:rowOff>76320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>167400</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>91800</xdr:rowOff>
+      <xdr:rowOff>118080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -690,8 +735,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4268880" y="5679360"/>
-          <a:ext cx="360" cy="42120"/>
+          <a:off x="4275360" y="5679360"/>
+          <a:ext cx="360" cy="41760"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -723,9 +768,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>498240</xdr:colOff>
+      <xdr:colOff>497880</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>69120</xdr:rowOff>
+      <xdr:rowOff>97920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -734,8 +779,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1922400" y="4853880"/>
-          <a:ext cx="1036800" cy="1010160"/>
+          <a:off x="1924920" y="4853880"/>
+          <a:ext cx="1037880" cy="1009800"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -767,9 +812,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>300240</xdr:colOff>
+      <xdr:colOff>299880</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>119160</xdr:rowOff>
+      <xdr:rowOff>118800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -778,8 +823,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1662120" y="4644720"/>
-          <a:ext cx="278640" cy="262080"/>
+          <a:off x="1664640" y="4644720"/>
+          <a:ext cx="278280" cy="261720"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -806,14 +851,14 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>63000</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>159840</xdr:rowOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>23760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>341640</xdr:colOff>
+      <xdr:colOff>341280</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>91800</xdr:rowOff>
+      <xdr:rowOff>120600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -822,8 +867,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1703520" y="5789520"/>
-          <a:ext cx="278640" cy="262080"/>
+          <a:off x="1706040" y="5789520"/>
+          <a:ext cx="278280" cy="261720"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -850,14 +895,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>448200</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>148680</xdr:rowOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>12600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>726840</xdr:colOff>
+      <xdr:colOff>726480</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>80640</xdr:rowOff>
+      <xdr:rowOff>109440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -866,8 +911,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2909160" y="5778360"/>
-          <a:ext cx="278640" cy="262080"/>
+          <a:off x="2913120" y="5778360"/>
+          <a:ext cx="278280" cy="261720"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -899,9 +944,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>736920</xdr:colOff>
+      <xdr:colOff>736560</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>9000</xdr:rowOff>
+      <xdr:rowOff>8640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -910,8 +955,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2919240" y="4699800"/>
-          <a:ext cx="278640" cy="262080"/>
+          <a:off x="2923200" y="4699800"/>
+          <a:ext cx="278280" cy="261720"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -945,10 +990,10 @@
   <dimension ref="B28:P48"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N32" activeCellId="0" sqref="N32"/>
+      <selection pane="topLeft" activeCell="K40" activeCellId="0" sqref="K40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="28" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H28" s="1" t="s">
@@ -1019,17 +1064,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="13.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="12"/>
       <c r="D31" s="11"/>
-      <c r="G31" s="7" t="s">
-        <v>10</v>
-      </c>
+      <c r="G31" s="7"/>
       <c r="H31" s="14" t="n">
         <v>36</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J31" s="15" t="n">
         <v>14</v>
@@ -1038,26 +1081,24 @@
         <v>4</v>
       </c>
       <c r="N31" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O31" s="16" t="n">
         <v>1</v>
       </c>
       <c r="P31" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="12"/>
       <c r="D32" s="11"/>
-      <c r="G32" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="G32" s="7"/>
       <c r="H32" s="14" t="n">
         <v>39</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J32" s="15" t="n">
         <v>12</v>
@@ -1065,77 +1106,71 @@
       <c r="M32" s="13" t="n">
         <v>0</v>
       </c>
-      <c r="N32" s="7" t="s">
-        <v>16</v>
-      </c>
+      <c r="N32" s="7"/>
       <c r="O32" s="16" t="n">
         <v>3</v>
       </c>
       <c r="P32" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C33" s="12"/>
       <c r="D33" s="11"/>
       <c r="E33" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G33" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H33" s="17" t="n">
+        <v>16</v>
+      </c>
+      <c r="G33" s="7"/>
+      <c r="H33" s="14" t="n">
         <v>34</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M33" s="18" t="n">
+      <c r="M33" s="14" t="n">
         <v>2</v>
       </c>
       <c r="O33" s="10" t="n">
         <v>21</v>
       </c>
       <c r="P33" s="11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="13.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="12"/>
       <c r="D34" s="11"/>
-      <c r="G34" s="7" t="s">
-        <v>22</v>
-      </c>
+      <c r="G34" s="7"/>
       <c r="H34" s="14" t="n">
         <v>35</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="J34" s="10" t="n">
         <v>13</v>
       </c>
-      <c r="M34" s="18" t="n">
+      <c r="M34" s="17" t="n">
         <v>15</v>
       </c>
-      <c r="N34" s="19" t="s">
-        <v>24</v>
+      <c r="N34" s="18" t="s">
+        <v>19</v>
       </c>
       <c r="O34" s="9" t="s">
         <v>3</v>
       </c>
       <c r="P34" s="11"/>
     </row>
-    <row r="35" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="12"/>
       <c r="D35" s="11"/>
       <c r="G35" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H35" s="14" t="n">
+        <v>20</v>
+      </c>
+      <c r="H35" s="19" t="n">
         <v>32</v>
       </c>
       <c r="J35" s="20" t="n">
@@ -1148,20 +1183,20 @@
         <v>19</v>
       </c>
       <c r="P35" s="11" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="7" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C36" s="12"/>
       <c r="D36" s="11"/>
       <c r="E36" s="7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="H36" s="10" t="n">
         <v>33</v>
@@ -1176,14 +1211,14 @@
         <v>18</v>
       </c>
       <c r="P36" s="11" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="21"/>
       <c r="D37" s="22"/>
       <c r="G37" s="7" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="H37" s="8" t="n">
         <v>25</v>
@@ -1202,70 +1237,109 @@
         <v>5</v>
       </c>
       <c r="P37" s="22" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="13.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="24" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="H39" s="25"/>
       <c r="I39" s="7" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H40" s="26"/>
+      <c r="O39" s="26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H40" s="27"/>
       <c r="I40" s="7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H41" s="27"/>
+      <c r="O40" s="26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H41" s="28"/>
       <c r="I41" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="O41" s="26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H42" s="29"/>
+      <c r="I42" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="O42" s="30" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="42" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H42" s="28"/>
-      <c r="I42" s="7" t="s">
+      <c r="P42" s="0" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H43" s="29"/>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H43" s="31"/>
       <c r="I43" s="7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="44" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H44" s="30"/>
+      <c r="O43" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="P43" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H44" s="32"/>
       <c r="I44" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H45" s="31"/>
+        <v>39</v>
+      </c>
+      <c r="O44" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="P44" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H45" s="33"/>
       <c r="I45" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H46" s="32"/>
+        <v>42</v>
+      </c>
+      <c r="O45" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="P45" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H46" s="34"/>
       <c r="I46" s="7" t="s">
-        <v>39</v>
+        <v>45</v>
+      </c>
+      <c r="O46" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="P46" s="0" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H47" s="33"/>
+      <c r="H47" s="35"/>
       <c r="I47" s="7" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H48" s="34"/>
+      <c r="H48" s="36"/>
       <c r="I48" s="7" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
i did a lot of things - fixed crash when loading games with the nes app - added new pcb that isn't finished yet - pinout changes?
</commit_message>
<xml_diff>
--- a/extras/pinout.xlsx
+++ b/extras/pinout.xlsx
@@ -20,7 +20,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="57">
+  <si>
+    <t xml:space="preserve">watch2 pinout guide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">by atctwo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESP32 WROVER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 way navigation switch</t>
+  </si>
   <si>
     <t xml:space="preserve">GND</t>
   </si>
@@ -112,6 +124,9 @@
     <t xml:space="preserve">reset</t>
   </si>
   <si>
+    <t xml:space="preserve">I2S DIN</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="10"/>
@@ -223,7 +238,13 @@
     <t xml:space="preserve">other peripherals</t>
   </si>
   <si>
+    <t xml:space="preserve">MCP23008</t>
+  </si>
+  <si>
     <t xml:space="preserve">Serial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">input only pins</t>
   </si>
 </sst>
 </file>
@@ -233,7 +254,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -256,6 +277,20 @@
       <family val="0"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
@@ -263,6 +298,7 @@
       <charset val="1"/>
     </font>
     <font>
+      <i val="true"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -270,8 +306,8 @@
       <charset val="1"/>
     </font>
     <font>
-      <i val="true"/>
       <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -455,8 +491,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="41">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -468,7 +516,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -512,7 +560,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -524,15 +576,19 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -552,15 +608,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -683,13 +735,13 @@
       <xdr:col>10</xdr:col>
       <xdr:colOff>46800</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>32760</xdr:rowOff>
+      <xdr:rowOff>37800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>753120</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>164520</xdr:rowOff>
+      <xdr:colOff>752760</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>16920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -702,8 +754,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8263440" y="4490280"/>
-          <a:ext cx="1528200" cy="1604880"/>
+          <a:off x="8269920" y="4490280"/>
+          <a:ext cx="1528200" cy="1604520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -720,13 +772,13 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>167040</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>76320</xdr:rowOff>
+      <xdr:rowOff>88920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>167400</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>118080</xdr:rowOff>
+      <xdr:rowOff>130320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -735,8 +787,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4275360" y="5679360"/>
-          <a:ext cx="360" cy="41760"/>
+          <a:off x="4278600" y="5679360"/>
+          <a:ext cx="360" cy="41400"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -764,13 +816,13 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>281880</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>66240</xdr:rowOff>
+      <xdr:rowOff>76320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>497880</xdr:colOff>
+      <xdr:colOff>497520</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>97920</xdr:rowOff>
+      <xdr:rowOff>110520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -779,8 +831,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1924920" y="4853880"/>
-          <a:ext cx="1037880" cy="1009800"/>
+          <a:off x="1926360" y="4853880"/>
+          <a:ext cx="1037880" cy="1009440"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -808,13 +860,13 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>21600</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>21960</xdr:rowOff>
+      <xdr:rowOff>29880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>299880</xdr:colOff>
+      <xdr:colOff>299520</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>118800</xdr:rowOff>
+      <xdr:rowOff>128520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -823,8 +875,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1664640" y="4644720"/>
-          <a:ext cx="278280" cy="261720"/>
+          <a:off x="1666080" y="4644720"/>
+          <a:ext cx="277920" cy="261360"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -852,13 +904,13 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>63000</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>23760</xdr:rowOff>
+      <xdr:rowOff>36720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>341280</xdr:colOff>
+      <xdr:colOff>340920</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>120600</xdr:rowOff>
+      <xdr:rowOff>135360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -867,8 +919,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1706040" y="5789520"/>
-          <a:ext cx="278280" cy="261720"/>
+          <a:off x="1707480" y="5789520"/>
+          <a:ext cx="277920" cy="261360"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -896,13 +948,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>448200</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>12600</xdr:rowOff>
+      <xdr:rowOff>25560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>726480</xdr:colOff>
+      <xdr:colOff>726120</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>109440</xdr:rowOff>
+      <xdr:rowOff>124200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -911,8 +963,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2913120" y="5778360"/>
-          <a:ext cx="278280" cy="261720"/>
+          <a:off x="2914920" y="5778360"/>
+          <a:ext cx="277920" cy="261360"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -940,13 +992,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>458280</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>77040</xdr:rowOff>
+      <xdr:rowOff>84960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>736560</xdr:colOff>
+      <xdr:colOff>736200</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>8640</xdr:rowOff>
+      <xdr:rowOff>20880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -955,8 +1007,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2923200" y="4699800"/>
-          <a:ext cx="278280" cy="261720"/>
+          <a:off x="2925000" y="4699800"/>
+          <a:ext cx="277920" cy="261360"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -987,359 +1039,390 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B28:P48"/>
+  <dimension ref="B19:P49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M41" activeCellId="0" sqref="M41"/>
+      <selection pane="topLeft" activeCell="L40" activeCellId="0" sqref="L40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="28" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H28" s="1" t="s">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I28" s="2"/>
-      <c r="J28" s="1" t="s">
+    </row>
+    <row r="20" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K27" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G28" s="3"/>
+      <c r="H28" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I28" s="5"/>
+      <c r="J28" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="N28" s="5"/>
+      <c r="O28" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="P28" s="7"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C29" s="8"/>
+      <c r="D29" s="7"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I29" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="J29" s="11" t="n">
+        <v>26</v>
+      </c>
+      <c r="M29" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="O29" s="13" t="n">
+        <v>23</v>
+      </c>
+      <c r="P29" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" s="15"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G30" s="3"/>
+      <c r="H30" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="I30" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J30" s="11" t="n">
+        <v>27</v>
+      </c>
+      <c r="M30" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="O30" s="13" t="n">
+        <v>22</v>
+      </c>
+      <c r="P30" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C31" s="15"/>
+      <c r="D31" s="14"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="18" t="n">
+        <v>36</v>
+      </c>
+      <c r="I31" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="J31" s="19" t="n">
+        <v>14</v>
+      </c>
+      <c r="M31" s="19" t="n">
+        <v>4</v>
+      </c>
+      <c r="N31" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="O31" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="P31" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C32" s="15"/>
+      <c r="D32" s="14"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="18" t="n">
+        <v>39</v>
+      </c>
+      <c r="I32" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J32" s="19" t="n">
+        <v>12</v>
+      </c>
+      <c r="M32" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
-      <c r="M28" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="N28" s="2"/>
-      <c r="O28" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="P28" s="4"/>
-    </row>
-    <row r="29" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="5"/>
-      <c r="D29" s="4"/>
-      <c r="H29" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="I29" s="7" t="s">
+      <c r="N32" s="10"/>
+      <c r="O32" s="20" t="n">
+        <v>3</v>
+      </c>
+      <c r="P32" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="15"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G33" s="17"/>
+      <c r="H33" s="18" t="n">
+        <v>34</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="M33" s="21" t="n">
         <v>2</v>
       </c>
-      <c r="J29" s="8" t="n">
+      <c r="O33" s="13" t="n">
+        <v>21</v>
+      </c>
+      <c r="P33" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C34" s="15"/>
+      <c r="D34" s="14"/>
+      <c r="G34" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="H34" s="22" t="n">
+        <v>35</v>
+      </c>
+      <c r="I34" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J34" s="13" t="n">
+        <v>13</v>
+      </c>
+      <c r="M34" s="23" t="n">
+        <v>15</v>
+      </c>
+      <c r="N34" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O34" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="P34" s="14"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C35" s="15"/>
+      <c r="D35" s="14"/>
+      <c r="G35" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H35" s="24" t="n">
+        <v>32</v>
+      </c>
+      <c r="J35" s="25" t="n">
+        <v>9</v>
+      </c>
+      <c r="M35" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O35" s="13" t="n">
+        <v>19</v>
+      </c>
+      <c r="P35" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="M29" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="O29" s="10" t="n">
-        <v>23</v>
-      </c>
-      <c r="P29" s="11" t="s">
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C36" s="15"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G36" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="H36" s="13" t="n">
+        <v>33</v>
+      </c>
+      <c r="J36" s="25" t="n">
+        <v>10</v>
+      </c>
+      <c r="M36" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O36" s="13" t="n">
+        <v>18</v>
+      </c>
+      <c r="P36" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C37" s="26"/>
+      <c r="D37" s="27"/>
+      <c r="G37" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="H37" s="11" t="n">
+        <v>25</v>
+      </c>
+      <c r="I37" s="28"/>
+      <c r="J37" s="25" t="n">
+        <v>11</v>
+      </c>
+      <c r="K37" s="28"/>
+      <c r="L37" s="28"/>
+      <c r="M37" s="25" t="n">
+        <v>6</v>
+      </c>
+      <c r="N37" s="28"/>
+      <c r="O37" s="13" t="n">
+        <v>5</v>
+      </c>
+      <c r="P37" s="27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="H39" s="30"/>
+      <c r="I39" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="7" t="s">
+      <c r="O39" s="17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H40" s="31"/>
+      <c r="I40" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="12"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="H30" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="I30" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="J30" s="8" t="n">
-        <v>27</v>
-      </c>
-      <c r="M30" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="O30" s="10" t="n">
-        <v>22</v>
-      </c>
-      <c r="P30" s="11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="12"/>
-      <c r="D31" s="11"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="14" t="n">
+      <c r="O40" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H41" s="32"/>
+      <c r="I41" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="I31" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="J31" s="15" t="n">
-        <v>14</v>
-      </c>
-      <c r="M31" s="15" t="n">
-        <v>4</v>
-      </c>
-      <c r="N31" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="O31" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="P31" s="11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="12"/>
-      <c r="D32" s="11"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="14" t="n">
+      <c r="O41" s="17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H42" s="33"/>
+      <c r="I42" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="O42" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="I32" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="J32" s="15" t="n">
-        <v>12</v>
-      </c>
-      <c r="M32" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="N32" s="7"/>
-      <c r="O32" s="16" t="n">
-        <v>3</v>
-      </c>
-      <c r="P32" s="11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C33" s="12"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G33" s="7"/>
-      <c r="H33" s="14" t="n">
-        <v>34</v>
-      </c>
-      <c r="J33" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M33" s="14" t="n">
-        <v>2</v>
-      </c>
-      <c r="O33" s="10" t="n">
-        <v>21</v>
-      </c>
-      <c r="P33" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C34" s="12"/>
-      <c r="D34" s="11"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="14" t="n">
-        <v>35</v>
-      </c>
-      <c r="I34" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="J34" s="10" t="n">
-        <v>13</v>
-      </c>
-      <c r="M34" s="17" t="n">
-        <v>15</v>
-      </c>
-      <c r="N34" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="O34" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="P34" s="11"/>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C35" s="12"/>
-      <c r="D35" s="11"/>
-      <c r="G35" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H35" s="19" t="n">
-        <v>32</v>
-      </c>
-      <c r="J35" s="20" t="n">
-        <v>9</v>
-      </c>
-      <c r="M35" s="20" t="n">
-        <v>8</v>
-      </c>
-      <c r="O35" s="10" t="n">
-        <v>19</v>
-      </c>
-      <c r="P35" s="11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C36" s="12"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G36" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H36" s="10" t="n">
-        <v>33</v>
-      </c>
-      <c r="J36" s="20" t="n">
-        <v>10</v>
-      </c>
-      <c r="M36" s="20" t="n">
-        <v>7</v>
-      </c>
-      <c r="O36" s="10" t="n">
-        <v>18</v>
-      </c>
-      <c r="P36" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C37" s="21"/>
-      <c r="D37" s="22"/>
-      <c r="G37" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="H37" s="8" t="n">
-        <v>25</v>
-      </c>
-      <c r="I37" s="23"/>
-      <c r="J37" s="20" t="n">
-        <v>11</v>
-      </c>
-      <c r="K37" s="23"/>
-      <c r="L37" s="23"/>
-      <c r="M37" s="20" t="n">
-        <v>6</v>
-      </c>
-      <c r="N37" s="23"/>
-      <c r="O37" s="10" t="n">
-        <v>5</v>
-      </c>
-      <c r="P37" s="22" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="H39" s="25"/>
-      <c r="I39" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="O39" s="26" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H40" s="27"/>
-      <c r="I40" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="O40" s="26" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H41" s="28"/>
-      <c r="I41" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O41" s="26" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H42" s="29"/>
-      <c r="I42" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="O42" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="P42" s="0" t="s">
-        <v>35</v>
+      <c r="P42" s="10" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H43" s="31"/>
-      <c r="I43" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="O43" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="P43" s="0" t="s">
-        <v>38</v>
+      <c r="H43" s="35"/>
+      <c r="I43" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="O43" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="P43" s="10" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H44" s="32"/>
-      <c r="I44" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="O44" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="P44" s="0" t="s">
-        <v>41</v>
+      <c r="H44" s="36"/>
+      <c r="I44" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="O44" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="P44" s="10" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H45" s="33"/>
-      <c r="I45" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="O45" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="P45" s="0" t="s">
-        <v>44</v>
+      <c r="H45" s="37"/>
+      <c r="I45" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="O45" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="P45" s="10" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H46" s="34"/>
-      <c r="I46" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="O46" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="P46" s="0" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H47" s="35"/>
-      <c r="I47" s="7" t="s">
-        <v>48</v>
+      <c r="H46" s="38"/>
+      <c r="I46" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="O46" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="P46" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H47" s="39"/>
+      <c r="I47" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="O47" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H48" s="36"/>
-      <c r="I48" s="7" t="s">
-        <v>49</v>
+      <c r="H48" s="40"/>
+      <c r="I48" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I49" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the system schematic it's mostly complete, i still need to do a bit of harware stuff to finish the prototype the schematic is based off the breadboard circuit i'm using to test the code
</commit_message>
<xml_diff>
--- a/extras/pinout.xlsx
+++ b/extras/pinout.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="59">
   <si>
     <t xml:space="preserve">watch2 pinout guide</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t xml:space="preserve">DC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wakeup</t>
   </si>
   <si>
     <r>
@@ -362,8 +365,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FF0000FF"/>
+        <bgColor rgb="FF0000FF"/>
       </patternFill>
     </fill>
     <fill>
@@ -380,6 +383,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFF1493"/>
         <bgColor rgb="FFFF00FF"/>
       </patternFill>
@@ -388,12 +397,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF00CED1"/>
         <bgColor rgb="FF33CCCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF0000FF"/>
-        <bgColor rgb="FF0000FF"/>
       </patternFill>
     </fill>
   </fills>
@@ -494,7 +497,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -567,7 +570,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -579,7 +582,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -587,15 +594,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -631,18 +638,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -651,7 +658,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -746,9 +753,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>752400</xdr:colOff>
+      <xdr:colOff>752040</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>16560</xdr:rowOff>
+      <xdr:rowOff>16200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -761,8 +768,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8282520" y="4490280"/>
-          <a:ext cx="1529280" cy="1604160"/>
+          <a:off x="8295120" y="4490280"/>
+          <a:ext cx="1530360" cy="1603800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -785,7 +792,7 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>167400</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>129960</xdr:rowOff>
+      <xdr:rowOff>129600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -794,8 +801,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4284720" y="5679360"/>
-          <a:ext cx="360" cy="41040"/>
+          <a:off x="4291200" y="5679360"/>
+          <a:ext cx="360" cy="40680"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -827,9 +834,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>497160</xdr:colOff>
+      <xdr:colOff>496800</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>110160</xdr:rowOff>
+      <xdr:rowOff>109800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -838,8 +845,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1928880" y="4853880"/>
-          <a:ext cx="1038960" cy="1009080"/>
+          <a:off x="1931400" y="4853880"/>
+          <a:ext cx="1039680" cy="1008720"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -871,9 +878,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>299160</xdr:colOff>
+      <xdr:colOff>298800</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>128160</xdr:rowOff>
+      <xdr:rowOff>127800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -882,8 +889,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1668600" y="4644720"/>
-          <a:ext cx="277560" cy="261000"/>
+          <a:off x="1671120" y="4644720"/>
+          <a:ext cx="277200" cy="260640"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -915,9 +922,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>340560</xdr:colOff>
+      <xdr:colOff>340200</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>135000</xdr:rowOff>
+      <xdr:rowOff>134640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -926,8 +933,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1710000" y="5789520"/>
-          <a:ext cx="277560" cy="261000"/>
+          <a:off x="1712520" y="5789520"/>
+          <a:ext cx="277200" cy="260640"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -959,9 +966,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>725760</xdr:colOff>
+      <xdr:colOff>725400</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>123840</xdr:rowOff>
+      <xdr:rowOff>123480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -970,8 +977,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2918880" y="5778360"/>
-          <a:ext cx="277560" cy="261000"/>
+          <a:off x="2922480" y="5778360"/>
+          <a:ext cx="277200" cy="260640"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -1003,9 +1010,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>735840</xdr:colOff>
+      <xdr:colOff>735480</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>20520</xdr:rowOff>
+      <xdr:rowOff>20160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1014,8 +1021,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2928960" y="4699800"/>
-          <a:ext cx="277560" cy="261000"/>
+          <a:off x="2932560" y="4699800"/>
+          <a:ext cx="277200" cy="260640"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -1049,10 +1056,10 @@
   <dimension ref="B19:P49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L42" activeCellId="0" sqref="L42"/>
+      <selection pane="topLeft" activeCell="H31" activeCellId="0" sqref="H31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="1" t="s">
@@ -1147,12 +1154,14 @@
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="15"/>
       <c r="D31" s="14"/>
-      <c r="G31" s="17"/>
+      <c r="G31" s="17" t="s">
+        <v>14</v>
+      </c>
       <c r="H31" s="18" t="n">
         <v>36</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J31" s="19" t="n">
         <v>14</v>
@@ -1161,24 +1170,24 @@
         <v>4</v>
       </c>
       <c r="N31" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O31" s="20" t="n">
         <v>1</v>
       </c>
       <c r="P31" s="14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="15"/>
       <c r="D32" s="14"/>
       <c r="G32" s="17"/>
-      <c r="H32" s="18" t="n">
+      <c r="H32" s="21" t="n">
         <v>39</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J32" s="19" t="n">
         <v>12</v>
@@ -1191,55 +1200,55 @@
         <v>3</v>
       </c>
       <c r="P32" s="14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C33" s="15"/>
       <c r="D33" s="14"/>
       <c r="E33" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G33" s="17"/>
-      <c r="H33" s="18" t="n">
+      <c r="H33" s="21" t="n">
         <v>34</v>
       </c>
       <c r="J33" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="M33" s="21" t="n">
+      <c r="M33" s="22" t="n">
         <v>2</v>
       </c>
       <c r="O33" s="13" t="n">
         <v>21</v>
       </c>
       <c r="P33" s="14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="15"/>
       <c r="D34" s="14"/>
       <c r="G34" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="H34" s="22" t="n">
+        <v>23</v>
+      </c>
+      <c r="H34" s="23" t="n">
         <v>35</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J34" s="13" t="n">
         <v>13</v>
       </c>
-      <c r="M34" s="23" t="n">
+      <c r="M34" s="24" t="n">
         <v>15</v>
       </c>
       <c r="N34" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O34" s="12" t="s">
         <v>7</v>
@@ -1250,189 +1259,189 @@
       <c r="C35" s="15"/>
       <c r="D35" s="14"/>
       <c r="G35" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="H35" s="24" t="n">
+        <v>26</v>
+      </c>
+      <c r="H35" s="25" t="n">
         <v>32</v>
       </c>
-      <c r="J35" s="25" t="n">
+      <c r="J35" s="26" t="n">
         <v>9</v>
       </c>
-      <c r="M35" s="25" t="n">
+      <c r="M35" s="26" t="n">
         <v>8</v>
       </c>
       <c r="O35" s="13" t="n">
         <v>19</v>
       </c>
       <c r="P35" s="14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C36" s="15"/>
       <c r="D36" s="14"/>
       <c r="E36" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G36" s="17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H36" s="13" t="n">
         <v>33</v>
       </c>
-      <c r="J36" s="25" t="n">
+      <c r="J36" s="26" t="n">
         <v>10</v>
       </c>
-      <c r="M36" s="25" t="n">
+      <c r="M36" s="26" t="n">
         <v>7</v>
       </c>
       <c r="O36" s="13" t="n">
         <v>18</v>
       </c>
       <c r="P36" s="14" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C37" s="26"/>
-      <c r="D37" s="27"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="28"/>
       <c r="G37" s="17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H37" s="11" t="n">
         <v>25</v>
       </c>
-      <c r="I37" s="28"/>
-      <c r="J37" s="25" t="n">
+      <c r="I37" s="29"/>
+      <c r="J37" s="26" t="n">
         <v>11</v>
       </c>
-      <c r="K37" s="28"/>
-      <c r="L37" s="28"/>
-      <c r="M37" s="25" t="n">
+      <c r="K37" s="29"/>
+      <c r="L37" s="29"/>
+      <c r="M37" s="26" t="n">
         <v>6</v>
       </c>
-      <c r="N37" s="28"/>
+      <c r="N37" s="29"/>
       <c r="O37" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="P37" s="27" t="s">
-        <v>32</v>
+      <c r="P37" s="28" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="H39" s="30"/>
+      <c r="B39" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="H39" s="31"/>
       <c r="I39" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="O39" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="P39" s="0" t="s">
+      <c r="O39" s="32" t="s">
         <v>35</v>
       </c>
+      <c r="P39" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H40" s="32"/>
+      <c r="H40" s="33"/>
       <c r="I40" s="2" t="s">
         <v>5</v>
       </c>
       <c r="O40" s="17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H41" s="33"/>
+      <c r="H41" s="34"/>
       <c r="I41" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="O41" s="17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H42" s="34"/>
+      <c r="H42" s="35"/>
       <c r="I42" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="O42" s="35" t="s">
         <v>40</v>
       </c>
+      <c r="O42" s="36" t="s">
+        <v>41</v>
+      </c>
       <c r="P42" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H43" s="36"/>
+      <c r="H43" s="37"/>
       <c r="I43" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="O43" s="35" t="s">
         <v>43</v>
       </c>
+      <c r="O43" s="36" t="s">
+        <v>44</v>
+      </c>
       <c r="P43" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H44" s="37"/>
+      <c r="H44" s="38"/>
       <c r="I44" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="O44" s="35" t="s">
         <v>46</v>
       </c>
+      <c r="O44" s="36" t="s">
+        <v>47</v>
+      </c>
       <c r="P44" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H45" s="38"/>
+      <c r="H45" s="39"/>
       <c r="I45" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="O45" s="35" t="s">
         <v>49</v>
       </c>
+      <c r="O45" s="36" t="s">
+        <v>50</v>
+      </c>
       <c r="P45" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H46" s="39"/>
+      <c r="H46" s="40"/>
       <c r="I46" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="O46" s="35" t="s">
         <v>52</v>
       </c>
+      <c r="O46" s="36" t="s">
+        <v>53</v>
+      </c>
       <c r="P46" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H47" s="40"/>
+      <c r="H47" s="41"/>
       <c r="I47" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="O47" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H48" s="41"/>
+      <c r="H48" s="42"/>
       <c r="I48" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I49" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>